<commit_message>
Content updates and restructuring
</commit_message>
<xml_diff>
--- a/chapters.xlsx
+++ b/chapters.xlsx
@@ -231,12 +231,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>CourseOverview</t>
-  </si>
-  <si>
-    <t>CourseResources</t>
-  </si>
-  <si>
     <t>Lecture</t>
   </si>
   <si>
@@ -301,6 +295,12 @@
   </si>
   <si>
     <t>Integration3LabExercises</t>
+  </si>
+  <si>
+    <t>ModuleOverview</t>
+  </si>
+  <si>
+    <t>ModuleResources</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,25 +1128,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1158,7 +1158,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1170,7 +1170,7 @@
         <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>IF(ISBLANK(A2),C2&amp;"."&amp;E2&amp;"."&amp;B2&amp;".md",C2&amp;"."&amp;E2&amp;"."&amp;RIGHT(B2,LEN(B2)-5))</f>
@@ -1188,7 +1188,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -1200,11 +1200,11 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G37" si="0">IF(ISBLANK(A3),C3&amp;"."&amp;E3&amp;"."&amp;B3&amp;".md",C3&amp;"."&amp;E3&amp;"."&amp;RIGHT(B3,LEN(B3)-5))</f>
-        <v>0.01.CourseOverview.md</v>
+        <v>0.01.ModuleOverview.md</v>
       </c>
       <c r="H3" s="2" t="str">
         <f t="shared" ref="H3:H50" si="1">IF(ISBLANK(A3),"",A3&amp;"/"&amp;B3)</f>
@@ -1212,13 +1212,13 @@
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I50" si="2">F3&amp;"/"&amp;G3</f>
-        <v>Integration0About/0.01.CourseOverview.md</v>
+        <v>Integration0About/0.01.ModuleOverview.md</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -1230,11 +1230,11 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0.02.CourseResources.md</v>
+        <v>0.02.ModuleResources.md</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1242,13 +1242,13 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Integration0About/0.02.CourseResources.md</v>
+        <v>Integration0About/0.02.ModuleResources.md</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>65</v>
@@ -1260,7 +1260,7 @@
         <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1274,7 +1274,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>65</v>
@@ -1286,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1318,7 +1318,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1350,7 +1350,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1382,7 +1382,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>66</v>
@@ -1411,7 +1411,7 @@
         <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1443,7 +1443,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1475,7 +1475,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1507,7 +1507,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1539,7 +1539,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1571,7 +1571,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1603,7 +1603,7 @@
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1635,7 +1635,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1667,7 +1667,7 @@
         <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1699,7 +1699,7 @@
         <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1731,7 +1731,7 @@
         <v>29</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1763,7 +1763,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1795,7 +1795,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1827,7 +1827,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1859,7 +1859,7 @@
         <v>32</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1891,7 +1891,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1923,7 +1923,7 @@
         <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1955,7 +1955,7 @@
         <v>49</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1987,7 +1987,7 @@
         <v>50</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2019,7 +2019,7 @@
         <v>51</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2051,7 +2051,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2083,7 +2083,7 @@
         <v>53</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2115,7 +2115,7 @@
         <v>54</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2144,10 +2144,10 @@
         <v>65</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2176,10 +2176,10 @@
         <v>65</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2208,10 +2208,10 @@
         <v>65</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>69</v>
@@ -2240,7 +2240,7 @@
         <v>68</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G36" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>69</v>
@@ -2269,7 +2269,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G37" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2301,7 +2301,7 @@
         <v>21</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G38" s="2" t="str">
         <f t="shared" ref="G38:G50" si="3">IF(ISBLANK(A38),C38&amp;"."&amp;E38&amp;"."&amp;B38&amp;".md",C38&amp;"."&amp;E38&amp;"."&amp;RIGHT(B38,LEN(B38)-2))</f>
@@ -2333,7 +2333,7 @@
         <v>22</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G39" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2365,7 +2365,7 @@
         <v>23</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G40" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2397,7 +2397,7 @@
         <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G41" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2415,7 +2415,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>69</v>
@@ -2427,7 +2427,7 @@
         <v>25</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G42" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2455,7 +2455,7 @@
         <v>26</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G43" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2487,7 +2487,7 @@
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G44" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2519,7 +2519,7 @@
         <v>28</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G45" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2551,7 +2551,7 @@
         <v>29</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2583,7 +2583,7 @@
         <v>20</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G47" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2615,7 +2615,7 @@
         <v>30</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G48" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>69</v>
@@ -2644,7 +2644,7 @@
         <v>31</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G49" s="2" t="str">
         <f t="shared" ref="G49" si="4">IF(ISBLANK(A49),C49&amp;"."&amp;E49&amp;"."&amp;B49&amp;".md",C49&amp;"."&amp;E49&amp;"."&amp;RIGHT(B49,LEN(B49)-2))</f>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>69</v>
@@ -2673,7 +2673,7 @@
         <v>32</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G50" s="2" t="str">
         <f t="shared" si="3"/>

</xml_diff>